<commit_message>
finalização do indicador de desempenho - densidade de defeito
</commit_message>
<xml_diff>
--- a/doc/Atividades Frade v10.xlsx
+++ b/doc/Atividades Frade v10.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>Extrações de dados do  SGQ, para acompanhamento das janelas de mudança semanais (Fernando Machado)</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Criar na cadeia puxada, gráfico CFD</t>
   </si>
   <si>
-    <t>Criar Indicador de desempenho - Taxa de Defeitos Atendidos no Prazo</t>
-  </si>
-  <si>
     <t>Criar nova opção no SGQ, para Indicadores de desempenho</t>
   </si>
   <si>
@@ -158,18 +155,24 @@
   </si>
   <si>
     <t>Migrar rotinas de carga do SGQ, para o servidor do TDM</t>
+  </si>
+  <si>
+    <t>Criar no SGQ, Indicadores de desempenho - Taxa de Defeitos dentrodo SLA</t>
+  </si>
+  <si>
+    <t>Criar no SGQ, Indicadores de desempenho - Densidade de Defeito</t>
   </si>
   <si>
     <t>Gustavo Já passou acesso ao servidor.
 Teste de conexão ao banco do ALM foi OK. 
-Faltar abrir GMUD para instação.</t>
+Faltar abrir GMUD para instação (aguardando João Andrés abrir GMUD).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +240,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -292,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -397,11 +408,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +716,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>27</v>
       </c>
@@ -724,74 +739,74 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="15">
-        <v>2</v>
-      </c>
-      <c r="D2" s="37">
-        <v>42998</v>
-      </c>
-      <c r="E2" s="36">
-        <v>0.5</v>
+        <v>35</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="18">
+        <v>43010</v>
+      </c>
+      <c r="E2" s="28">
+        <v>0.45</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>34</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="20">
+        <v>4</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="28">
-        <v>0.45</v>
+        <v>0.15</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>36</v>
       </c>
       <c r="G3" s="32"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C4" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="28">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C5" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="28">
@@ -802,15 +817,15 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C6" s="20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="28">
@@ -821,29 +836,21 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="20">
-        <v>7</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="28">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="15"/>
@@ -851,58 +858,67 @@
       <c r="F8" s="15"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="30"/>
+        <v>16</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="25" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="29">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="29">
+        <v>1</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -914,10 +930,10 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -929,10 +945,10 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="25" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -944,27 +960,27 @@
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="25" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="29">
-        <v>1</v>
-      </c>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="36">
+        <v>1</v>
+      </c>
+      <c r="F16" s="38" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="35"/>
+        <v>19</v>
+      </c>
+      <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="29">
         <v>1</v>
@@ -972,61 +988,61 @@
       <c r="F17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="15"/>
       <c r="E18" s="29">
         <v>1</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="27" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="29">
-        <v>1</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="25" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="29">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="29">
-        <v>1</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="22"/>
       <c r="E21" s="29">
         <v>1</v>
@@ -1034,14 +1050,12 @@
       <c r="F21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
       <c r="B22" s="25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="22"/>
@@ -1051,14 +1065,16 @@
       <c r="F22" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="G22" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="23"/>
+      <c r="B23" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="21"/>
       <c r="D23" s="22"/>
       <c r="E23" s="29">
         <v>1</v>
@@ -1066,14 +1082,12 @@
       <c r="F23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="26" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="22"/>
@@ -1083,12 +1097,14 @@
       <c r="F24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="10"/>
+      <c r="G24" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="26" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="22"/>
@@ -1098,12 +1114,12 @@
       <c r="F25" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="22"/>
@@ -1113,12 +1129,12 @@
       <c r="F26" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="10"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="23"/>
       <c r="D27" s="22"/>
@@ -1128,12 +1144,12 @@
       <c r="F27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
-      <c r="B28" s="26" t="s">
-        <v>1</v>
+      <c r="B28" s="39" t="s">
+        <v>23</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="22"/>
@@ -1143,16 +1159,31 @@
       <c r="F28" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="10"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="24"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="24"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>